<commit_message>
telecom lab experiment added
</commit_message>
<xml_diff>
--- a/lab_1_Traffic_simulation.xlsx
+++ b/lab_1_Traffic_simulation.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="2100" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -51,8 +51,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,13 +112,32 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -134,6 +153,7 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -148,6 +168,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$O$6:$O$21</c:f>
@@ -205,6 +226,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F199-4D93-A207-E7E3A539839D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -220,6 +246,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$P$6:$P$21</c:f>
@@ -277,7 +304,21 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F199-4D93-A207-E7E3A539839D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="70813184"/>
         <c:axId val="70814720"/>
       </c:barChart>
@@ -286,22 +327,29 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="70814720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="70814720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="70813184"/>
         <c:crosses val="autoZero"/>
@@ -310,9 +358,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -327,19 +377,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -400,7 +456,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -432,9 +488,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -466,6 +540,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -641,14 +733,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:P253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5:P21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
@@ -660,7 +752,7 @@
     <col min="15" max="16" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:16">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
@@ -682,7 +774,7 @@
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" spans="3:16">
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" s="5">
         <v>0.46852111470227698</v>
       </c>
@@ -711,7 +803,7 @@
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="3:16">
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="5">
         <v>7.9558986759264982E-3</v>
       </c>
@@ -752,7 +844,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="3:16">
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6" s="5">
         <v>0.43570965616074186</v>
       </c>
@@ -785,7 +877,7 @@
         <v>0</v>
       </c>
       <c r="N6" s="5">
-        <f>COUNTIF($K$5:$K$35,"="&amp;M6)</f>
+        <f t="shared" ref="N6:N21" si="2">COUNTIF($K$5:$K$35,"="&amp;M6)</f>
         <v>0</v>
       </c>
       <c r="O6" s="5">
@@ -797,7 +889,7 @@
         <v>2.4036947641951407E-4</v>
       </c>
     </row>
-    <row r="7" spans="3:16">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7" s="5">
         <v>9.5413897529229352E-2</v>
       </c>
@@ -822,7 +914,7 @@
         <v>29</v>
       </c>
       <c r="K7" s="5">
-        <f t="shared" ref="K7:K35" si="2">J7-J6</f>
+        <f t="shared" ref="K7:K35" si="3">J7-J6</f>
         <v>11</v>
       </c>
       <c r="L7" s="5"/>
@@ -830,11 +922,11 @@
         <v>1</v>
       </c>
       <c r="N7" s="5">
-        <f>COUNTIF($K$5:$K$35,"="&amp;M7)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O7" s="5">
-        <f t="shared" ref="O7:O21" si="3">N7/31</f>
+        <f>N7/31</f>
         <v>0</v>
       </c>
       <c r="P7" s="5">
@@ -842,7 +934,7 @@
         <v>2.0030789701626175E-3</v>
       </c>
     </row>
-    <row r="8" spans="3:16">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C8" s="5">
         <v>0.28339648241218929</v>
       </c>
@@ -867,7 +959,7 @@
         <v>40</v>
       </c>
       <c r="K8" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="L8" s="5"/>
@@ -875,11 +967,11 @@
         <v>2</v>
       </c>
       <c r="N8" s="5">
-        <f>COUNTIF($K$5:$K$35,"="&amp;M8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O8" s="5">
-        <f t="shared" si="3"/>
+        <f>N8/31</f>
         <v>0</v>
       </c>
       <c r="P8" s="5">
@@ -887,7 +979,7 @@
         <v>8.3461623756775731E-3</v>
       </c>
     </row>
-    <row r="9" spans="3:16">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C9" s="5">
         <v>0.43027378062804988</v>
       </c>
@@ -912,7 +1004,7 @@
         <v>45</v>
       </c>
       <c r="K9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="L9" s="5"/>
@@ -920,11 +1012,11 @@
         <v>3</v>
       </c>
       <c r="N9" s="5">
-        <f>COUNTIF($K$5:$K$35,"="&amp;M9)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O9" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="O7:O21" si="6">N9/31</f>
         <v>6.4516129032258063E-2</v>
       </c>
       <c r="P9" s="5">
@@ -932,7 +1024,7 @@
         <v>2.3183784376882149E-2</v>
       </c>
     </row>
-    <row r="10" spans="3:16">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C10" s="5">
         <v>0.66187405826371504</v>
       </c>
@@ -957,7 +1049,7 @@
         <v>54</v>
       </c>
       <c r="K10" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="L10" s="5"/>
@@ -965,11 +1057,11 @@
         <v>4</v>
       </c>
       <c r="N10" s="5">
-        <f>COUNTIF($K$5:$K$35,"="&amp;M10)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O10" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>9.6774193548387094E-2</v>
       </c>
       <c r="P10" s="5">
@@ -977,7 +1069,7 @@
         <v>4.8299550785171154E-2</v>
       </c>
     </row>
-    <row r="11" spans="3:16">
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C11" s="5">
         <v>0.25839337744705859</v>
       </c>
@@ -1002,7 +1094,7 @@
         <v>62</v>
       </c>
       <c r="K11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L11" s="5"/>
@@ -1010,11 +1102,11 @@
         <v>5</v>
       </c>
       <c r="N11" s="5">
-        <f>COUNTIF($K$5:$K$35,"="&amp;M11)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O11" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>9.6774193548387094E-2</v>
       </c>
       <c r="P11" s="5">
@@ -1022,7 +1114,7 @@
         <v>8.0499251308618583E-2</v>
       </c>
     </row>
-    <row r="12" spans="3:16">
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" s="5">
         <v>7.161398006668751E-2</v>
       </c>
@@ -1047,7 +1139,7 @@
         <v>66</v>
       </c>
       <c r="K12" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="L12" s="5"/>
@@ -1055,11 +1147,11 @@
         <v>6</v>
       </c>
       <c r="N12" s="5">
-        <f>COUNTIF($K$5:$K$35,"="&amp;M12)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O12" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.4516129032258063E-2</v>
       </c>
       <c r="P12" s="5">
@@ -1067,7 +1159,7 @@
         <v>0.11180451570641471</v>
       </c>
     </row>
-    <row r="13" spans="3:16">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C13" s="5">
         <v>5.5007309218872535E-2</v>
       </c>
@@ -1092,7 +1184,7 @@
         <v>75</v>
       </c>
       <c r="K13" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="L13" s="5"/>
@@ -1100,11 +1192,11 @@
         <v>7</v>
       </c>
       <c r="N13" s="5">
-        <f>COUNTIF($K$5:$K$35,"="&amp;M13)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O13" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>9.6774193548387094E-2</v>
       </c>
       <c r="P13" s="5">
@@ -1112,7 +1204,7 @@
         <v>0.13310061393620801</v>
       </c>
     </row>
-    <row r="14" spans="3:16">
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C14" s="5">
         <v>0.29886420867398655</v>
       </c>
@@ -1137,7 +1229,7 @@
         <v>83</v>
       </c>
       <c r="K14" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L14" s="5"/>
@@ -1145,11 +1237,11 @@
         <v>8</v>
       </c>
       <c r="N14" s="5">
-        <f>COUNTIF($K$5:$K$35,"="&amp;M14)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="O14" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.19354838709677419</v>
       </c>
       <c r="P14" s="5">
@@ -1157,7 +1249,7 @@
         <v>0.1386464728502167</v>
       </c>
     </row>
-    <row r="15" spans="3:16">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C15" s="5">
         <v>0.32900154999178399</v>
       </c>
@@ -1182,7 +1274,7 @@
         <v>93</v>
       </c>
       <c r="K15" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="L15" s="5"/>
@@ -1190,11 +1282,11 @@
         <v>9</v>
       </c>
       <c r="N15" s="5">
-        <f>COUNTIF($K$5:$K$35,"="&amp;M15)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.4516129032258063E-2</v>
       </c>
       <c r="P15" s="5">
@@ -1202,7 +1294,7 @@
         <v>0.12837636375020064</v>
       </c>
     </row>
-    <row r="16" spans="3:16">
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C16" s="5">
         <v>0.66369920181222164</v>
       </c>
@@ -1227,7 +1319,7 @@
         <v>104</v>
       </c>
       <c r="K16" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="L16" s="5"/>
@@ -1235,11 +1327,11 @@
         <v>10</v>
       </c>
       <c r="N16" s="5">
-        <f>COUNTIF($K$5:$K$35,"="&amp;M16)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O16" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.4516129032258063E-2</v>
       </c>
       <c r="P16" s="5">
@@ -1247,7 +1339,7 @@
         <v>0.10698030312516721</v>
       </c>
     </row>
-    <row r="17" spans="3:16">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
         <v>0.43227848377837752</v>
       </c>
@@ -1270,18 +1362,18 @@
         <v>116</v>
       </c>
       <c r="K17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="M17" s="1">
         <v>11</v>
       </c>
       <c r="N17" s="1">
-        <f>COUNTIF($K$5:$K$35,"="&amp;M17)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="O17" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.12903225806451613</v>
       </c>
       <c r="P17" s="1">
@@ -1289,7 +1381,7 @@
         <v>8.1045684185732741E-2</v>
       </c>
     </row>
-    <row r="18" spans="3:16">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
         <v>0.82807004380381888</v>
       </c>
@@ -1312,18 +1404,18 @@
         <v>126</v>
       </c>
       <c r="K18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="M18" s="1">
         <v>12</v>
       </c>
       <c r="N18" s="1">
-        <f>COUNTIF($K$5:$K$35,"="&amp;M18)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.2258064516129031E-2</v>
       </c>
       <c r="P18" s="1">
@@ -1331,7 +1423,7 @@
         <v>5.628172512898108E-2</v>
       </c>
     </row>
-    <row r="19" spans="3:16">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <v>0.98125308306867742</v>
       </c>
@@ -1354,18 +1446,18 @@
         <v>132</v>
       </c>
       <c r="K19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="M19" s="1">
         <v>13</v>
       </c>
       <c r="N19" s="1">
-        <f>COUNTIF($K$5:$K$35,"="&amp;M19)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.2258064516129031E-2</v>
       </c>
       <c r="P19" s="1">
@@ -1373,7 +1465,7 @@
         <v>3.6078028928834022E-2</v>
       </c>
     </row>
-    <row r="20" spans="3:16">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <v>0.71788672782063578</v>
       </c>
@@ -1396,18 +1488,18 @@
         <v>140</v>
       </c>
       <c r="K20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="M20" s="1">
         <v>14</v>
       </c>
       <c r="N20" s="1">
-        <f>COUNTIF($K$5:$K$35,"="&amp;M20)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.2258064516129031E-2</v>
       </c>
       <c r="P20" s="1">
@@ -1415,7 +1507,7 @@
         <v>2.1475017219544066E-2</v>
       </c>
     </row>
-    <row r="21" spans="3:16">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <v>0.40459646183680054</v>
       </c>
@@ -1438,18 +1530,18 @@
         <v>148</v>
       </c>
       <c r="K21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="M21" s="1">
         <v>15</v>
       </c>
       <c r="N21" s="1">
-        <f>COUNTIF($K$5:$K$35,"="&amp;M21)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.2258064516129031E-2</v>
       </c>
       <c r="P21" s="1">
@@ -1457,7 +1549,7 @@
         <v>1.1930565121968923E-2</v>
       </c>
     </row>
-    <row r="22" spans="3:16">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <v>0.95334953869349426</v>
       </c>
@@ -1480,7 +1572,7 @@
         <v>161</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="N22" s="1">
@@ -1488,7 +1580,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="3:16">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <v>0.1905706636151574</v>
       </c>
@@ -1511,11 +1603,11 @@
         <v>165</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="3:16">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <v>0.42262499985499336</v>
       </c>
@@ -1538,11 +1630,11 @@
         <v>170</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="3:16">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <v>0.30115626593712008</v>
       </c>
@@ -1565,11 +1657,11 @@
         <v>177</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="3:16">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <v>0.7929467664582468</v>
       </c>
@@ -1592,11 +1684,11 @@
         <v>188</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="3:16">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <v>0.77875379612813855</v>
       </c>
@@ -1619,11 +1711,11 @@
         <v>193</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="3:16">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
         <v>0.4240299811975099</v>
       </c>
@@ -1646,11 +1738,11 @@
         <v>197</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="3:16">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
         <v>0.7572693851936938</v>
       </c>
@@ -1673,11 +1765,11 @@
         <v>205</v>
       </c>
       <c r="K29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="3:16">
+    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
         <v>2.0422323338842308E-3</v>
       </c>
@@ -1700,11 +1792,11 @@
         <v>212</v>
       </c>
       <c r="K30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="3:16">
+    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
         <v>0.42344011476169108</v>
       </c>
@@ -1727,11 +1819,11 @@
         <v>218</v>
       </c>
       <c r="K31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="3:16">
+    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
         <v>0.73392208048698304</v>
       </c>
@@ -1754,11 +1846,11 @@
         <v>226</v>
       </c>
       <c r="K32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="3:11">
+    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
         <v>0.51432230380276267</v>
       </c>
@@ -1781,11 +1873,11 @@
         <v>240</v>
       </c>
       <c r="K33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="3:11">
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <v>7.2094347382877011E-2</v>
       </c>
@@ -1808,11 +1900,11 @@
         <v>247</v>
       </c>
       <c r="K34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="3:11">
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <v>0.55696307986668825</v>
       </c>
@@ -1835,11 +1927,11 @@
         <v>250</v>
       </c>
       <c r="K35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="3:11">
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
         <v>0.59818793071617726</v>
       </c>
@@ -1852,7 +1944,7 @@
         <v>327.45902901180995</v>
       </c>
     </row>
-    <row r="37" spans="3:11">
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <v>0.12404932456397222</v>
       </c>
@@ -1865,7 +1957,7 @@
         <v>329.0483749663407</v>
       </c>
     </row>
-    <row r="38" spans="3:11">
+    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
         <v>0.82590058230134766</v>
       </c>
@@ -1878,7 +1970,7 @@
         <v>350.02592028855094</v>
       </c>
     </row>
-    <row r="39" spans="3:11">
+    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
         <v>0.51326286891805095</v>
       </c>
@@ -1891,7 +1983,7 @@
         <v>358.66629317096488</v>
       </c>
     </row>
-    <row r="40" spans="3:11">
+    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <v>0.51238042306634068</v>
       </c>
@@ -1904,7 +1996,7 @@
         <v>367.2849299622149</v>
       </c>
     </row>
-    <row r="41" spans="3:11">
+    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
         <v>0.15375561187726117</v>
       </c>
@@ -1917,7 +2009,7 @@
         <v>369.28829499712668</v>
       </c>
     </row>
-    <row r="42" spans="3:11">
+    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
         <v>0.27617929346014414</v>
       </c>
@@ -1930,7 +2022,7 @@
         <v>373.16683371911557</v>
       </c>
     </row>
-    <row r="43" spans="3:11">
+    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
         <v>0.24819677646773863</v>
       </c>
@@ -1943,7 +2035,7 @@
         <v>376.5902016404217</v>
       </c>
     </row>
-    <row r="44" spans="3:11">
+    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
         <v>0.92696348186844002</v>
       </c>
@@ -1956,7 +2048,7 @@
         <v>407.99175021488634</v>
       </c>
     </row>
-    <row r="45" spans="3:11">
+    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
         <v>0.44137135202410072</v>
       </c>
@@ -1969,7 +2061,7 @@
         <v>414.97899431256241</v>
       </c>
     </row>
-    <row r="46" spans="3:11">
+    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
         <v>0.16984753128978358</v>
       </c>
@@ -1982,7 +2074,7 @@
         <v>417.21274508640892</v>
       </c>
     </row>
-    <row r="47" spans="3:11">
+    <row r="47" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
         <v>0.95522370398530709</v>
       </c>
@@ -1995,7 +2087,7 @@
         <v>454.48566172323882</v>
       </c>
     </row>
-    <row r="48" spans="3:11">
+    <row r="48" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
         <v>0.96056018940607246</v>
       </c>
@@ -2008,7 +2100,7 @@
         <v>493.28141634297208</v>
       </c>
     </row>
-    <row r="49" spans="3:5">
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
         <v>0.54807518957870127</v>
       </c>
@@ -2021,7 +2113,7 @@
         <v>502.8122898823259</v>
       </c>
     </row>
-    <row r="50" spans="3:5">
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
         <v>0.27519624453440628</v>
       </c>
@@ -2034,7 +2126,7 @@
         <v>506.6745419969447</v>
       </c>
     </row>
-    <row r="51" spans="3:5">
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
         <v>0.49269253829791704</v>
       </c>
@@ -2047,7 +2139,7 @@
         <v>514.81819830726351</v>
       </c>
     </row>
-    <row r="52" spans="3:5">
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
         <v>0.5478115683917153</v>
       </c>
@@ -2060,7 +2152,7 @@
         <v>524.34207393045722</v>
       </c>
     </row>
-    <row r="53" spans="3:5">
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
         <v>0.95071548196886635</v>
       </c>
@@ -2073,7 +2165,7 @@
         <v>560.46381732804991</v>
       </c>
     </row>
-    <row r="54" spans="3:5">
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
         <v>0.55774577489416011</v>
       </c>
@@ -2086,7 +2178,7 @@
         <v>570.2542620359925</v>
       </c>
     </row>
-    <row r="55" spans="3:5">
+    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
         <v>0.68890967370145351</v>
       </c>
@@ -2099,7 +2191,7 @@
         <v>584.26632568454772</v>
       </c>
     </row>
-    <row r="56" spans="3:5">
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C56" s="1">
         <v>0.45547520902489236</v>
       </c>
@@ -2112,7 +2204,7 @@
         <v>591.56042737871644</v>
       </c>
     </row>
-    <row r="57" spans="3:5">
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C57" s="1">
         <v>0.32703091085818592</v>
       </c>
@@ -2125,7 +2217,7 @@
         <v>596.31309794285585</v>
       </c>
     </row>
-    <row r="58" spans="3:5">
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C58" s="1">
         <v>0.71085274240523444</v>
       </c>
@@ -2138,7 +2230,7 @@
         <v>611.20292808835597</v>
       </c>
     </row>
-    <row r="59" spans="3:5">
+    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C59" s="1">
         <v>0.38552956206468281</v>
       </c>
@@ -2151,7 +2243,7 @@
         <v>617.04686159207085</v>
       </c>
     </row>
-    <row r="60" spans="3:5">
+    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C60" s="1">
         <v>0.62211958442533621</v>
       </c>
@@ -2164,7 +2256,7 @@
         <v>628.72499152401656</v>
       </c>
     </row>
-    <row r="61" spans="3:5">
+    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C61" s="1">
         <v>0.92254017377667896</v>
       </c>
@@ -2177,7 +2269,7 @@
         <v>659.42094170404471</v>
       </c>
     </row>
-    <row r="62" spans="3:5">
+    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C62" s="1">
         <v>0.56720431711900954</v>
       </c>
@@ -2190,7 +2282,7 @@
         <v>669.47081602034905</v>
       </c>
     </row>
-    <row r="63" spans="3:5">
+    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C63" s="1">
         <v>0.24721285537747928</v>
       </c>
@@ -2203,7 +2295,7 @@
         <v>672.87848923163165</v>
       </c>
     </row>
-    <row r="64" spans="3:5">
+    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C64" s="1">
         <v>2.5820105090329948E-2</v>
       </c>
@@ -2216,7 +2308,7 @@
         <v>673.19240077596942</v>
       </c>
     </row>
-    <row r="65" spans="3:5">
+    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C65" s="1">
         <v>0.13890392991005407</v>
       </c>
@@ -2229,7 +2321,7 @@
         <v>674.9869911893594</v>
       </c>
     </row>
-    <row r="66" spans="3:5">
+    <row r="66" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C66" s="1">
         <v>0.91828372790906543</v>
       </c>
@@ -2242,7 +2334,7 @@
         <v>705.041016727135</v>
       </c>
     </row>
-    <row r="67" spans="3:5">
+    <row r="67" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C67" s="1">
         <v>0.85400455114478468</v>
       </c>
@@ -2255,7 +2347,7 @@
         <v>728.13117468694566</v>
       </c>
     </row>
-    <row r="68" spans="3:5">
+    <row r="68" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C68" s="1">
         <v>0.63664813004469334</v>
       </c>
@@ -2268,12 +2360,12 @@
         <v>740.2797775929796</v>
       </c>
     </row>
-    <row r="69" spans="3:5">
+    <row r="69" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C69" s="1">
         <v>0.96040893175530195</v>
       </c>
       <c r="D69">
-        <f t="shared" ref="D69:D132" si="6">-12*LN(1-C69)</f>
+        <f t="shared" ref="D69:D132" si="7">-12*LN(1-C69)</f>
         <v>38.749820826457203</v>
       </c>
       <c r="E69">
@@ -2281,2395 +2373,2395 @@
         <v>779.02959841943675</v>
       </c>
     </row>
-    <row r="70" spans="3:5">
+    <row r="70" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C70" s="1">
         <v>0.90562676807241971</v>
       </c>
       <c r="D70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>28.325973673567649</v>
       </c>
       <c r="E70">
-        <f t="shared" ref="E70:E133" si="7">D70+E69</f>
+        <f t="shared" ref="E70:E133" si="8">D70+E69</f>
         <v>807.35557209300441</v>
       </c>
     </row>
-    <row r="71" spans="3:5">
+    <row r="71" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C71" s="1">
         <v>0.39212224895551362</v>
       </c>
       <c r="D71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.9733778151251684</v>
       </c>
       <c r="E71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>813.32894990812963</v>
       </c>
     </row>
-    <row r="72" spans="3:5">
+    <row r="72" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C72" s="1">
         <v>0.13931599869860101</v>
       </c>
       <c r="D72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.800334266091218</v>
       </c>
       <c r="E72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>815.12928417422086</v>
       </c>
     </row>
-    <row r="73" spans="3:5">
+    <row r="73" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C73" s="1">
         <v>0.41739602993596625</v>
       </c>
       <c r="D73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.4829714410716015</v>
       </c>
       <c r="E73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>821.6122556152925</v>
       </c>
     </row>
-    <row r="74" spans="3:5">
+    <row r="74" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C74" s="1">
         <v>0.69958926519181763</v>
       </c>
       <c r="D74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14.431255496201128</v>
       </c>
       <c r="E74">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>836.04351111149367</v>
       </c>
     </row>
-    <row r="75" spans="3:5">
+    <row r="75" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C75" s="1">
         <v>0.18900779039809024</v>
       </c>
       <c r="D75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5139619699495048</v>
       </c>
       <c r="E75">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>838.55747308144316</v>
       </c>
     </row>
-    <row r="76" spans="3:5">
+    <row r="76" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C76" s="1">
         <v>0.76716632327719925</v>
       </c>
       <c r="D76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>17.489170969497874</v>
       </c>
       <c r="E76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>856.04664405094104</v>
       </c>
     </row>
-    <row r="77" spans="3:5">
+    <row r="77" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C77" s="1">
         <v>0.50423887604825435</v>
       </c>
       <c r="D77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.4199328784253424</v>
       </c>
       <c r="E77">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>864.4665769293664</v>
       </c>
     </row>
-    <row r="78" spans="3:5">
+    <row r="78" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C78" s="1">
         <v>0.57571988226728599</v>
       </c>
       <c r="D78">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10.288336642279893</v>
       </c>
       <c r="E78">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>874.75491357164628</v>
       </c>
     </row>
-    <row r="79" spans="3:5">
+    <row r="79" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C79" s="1">
         <v>0.97701554782479061</v>
       </c>
       <c r="D79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>45.27524740825271</v>
       </c>
       <c r="E79">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>920.03016097989894</v>
       </c>
     </row>
-    <row r="80" spans="3:5">
+    <row r="80" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C80" s="1">
         <v>0.82574551550411379</v>
       </c>
       <c r="D80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>20.966861924217593</v>
       </c>
       <c r="E80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>940.99702290411653</v>
       </c>
     </row>
-    <row r="81" spans="3:5">
+    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C81" s="1">
         <v>0.50427364242105277</v>
       </c>
       <c r="D81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.4207744351399221</v>
       </c>
       <c r="E81">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>949.41779733925648</v>
       </c>
     </row>
-    <row r="82" spans="3:5">
+    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C82" s="1">
         <v>0.10681319662829836</v>
       </c>
       <c r="D82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.3555144041065501</v>
       </c>
       <c r="E82">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>950.77331174336302</v>
       </c>
     </row>
-    <row r="83" spans="3:5">
+    <row r="83" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C83" s="1">
         <v>0.10238494793160235</v>
       </c>
       <c r="D83">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.2961677013907562</v>
       </c>
       <c r="E83">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>952.06947944475382</v>
       </c>
     </row>
-    <row r="84" spans="3:5">
+    <row r="84" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C84" s="1">
         <v>0.66415635365484471</v>
       </c>
       <c r="D84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13.093314786970158</v>
       </c>
       <c r="E84">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>965.16279423172398</v>
       </c>
     </row>
-    <row r="85" spans="3:5">
+    <row r="85" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C85" s="1">
         <v>0.14603815307247547</v>
       </c>
       <c r="D85">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.8944251430454155</v>
       </c>
       <c r="E85">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>967.05721937476937</v>
       </c>
     </row>
-    <row r="86" spans="3:5">
+    <row r="86" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C86" s="1">
         <v>0.77476030674159024</v>
       </c>
       <c r="D86">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>17.887081685279647</v>
       </c>
       <c r="E86">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>984.94430106004904</v>
       </c>
     </row>
-    <row r="87" spans="3:5">
+    <row r="87" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C87" s="1">
         <v>0.78758035583402486</v>
       </c>
       <c r="D87">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>18.590298086806165</v>
       </c>
       <c r="E87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1003.5345991468552</v>
       </c>
     </row>
-    <row r="88" spans="3:5">
+    <row r="88" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C88" s="1">
         <v>0.45778299443208659</v>
       </c>
       <c r="D88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.3450677407555123</v>
       </c>
       <c r="E88">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1010.8796668876107</v>
       </c>
     </row>
-    <row r="89" spans="3:5">
+    <row r="89" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C89" s="1">
         <v>0.39081160416890981</v>
       </c>
       <c r="D89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.947532476218341</v>
       </c>
       <c r="E89">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1016.8271993638291</v>
       </c>
     </row>
-    <row r="90" spans="3:5">
+    <row r="90" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C90" s="1">
         <v>0.83801214050257533</v>
       </c>
       <c r="D90">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>21.842806655183036</v>
       </c>
       <c r="E90">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1038.6700060190121</v>
       </c>
     </row>
-    <row r="91" spans="3:5">
+    <row r="91" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C91" s="1">
         <v>0.13623537206658565</v>
       </c>
       <c r="D91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.7574596239786473</v>
       </c>
       <c r="E91">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1040.4274656429907</v>
       </c>
     </row>
-    <row r="92" spans="3:5">
+    <row r="92" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C92" s="1">
         <v>0.88865035027155059</v>
       </c>
       <c r="D92">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>26.340960371573402</v>
       </c>
       <c r="E92">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1066.7684260145641</v>
       </c>
     </row>
-    <row r="93" spans="3:5">
+    <row r="93" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C93" s="1">
         <v>2.3016140916531924E-4</v>
       </c>
       <c r="D93">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.7622548044083997E-3</v>
       </c>
       <c r="E93">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1066.7711882693684</v>
       </c>
     </row>
-    <row r="94" spans="3:5">
+    <row r="94" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C94" s="1">
         <v>0.13201305138379604</v>
       </c>
       <c r="D94">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.698943207095337</v>
       </c>
       <c r="E94">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1068.4701314764636</v>
       </c>
     </row>
-    <row r="95" spans="3:5">
+    <row r="95" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C95" s="1">
         <v>0.68543753934352303</v>
       </c>
       <c r="D95">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13.878871434232234</v>
       </c>
       <c r="E95">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1082.3490029106958</v>
       </c>
     </row>
-    <row r="96" spans="3:5">
+    <row r="96" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C96" s="1">
         <v>0.70187919846652069</v>
       </c>
       <c r="D96">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14.523078004143176</v>
       </c>
       <c r="E96">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1096.872080914839</v>
       </c>
     </row>
-    <row r="97" spans="3:5">
+    <row r="97" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C97" s="1">
         <v>0.95710152541758231</v>
       </c>
       <c r="D97">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>37.787028134397005</v>
       </c>
       <c r="E97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1134.6591090492359</v>
       </c>
     </row>
-    <row r="98" spans="3:5">
+    <row r="98" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C98" s="1">
         <v>0.72041155604481899</v>
       </c>
       <c r="D98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>15.293239201308189</v>
       </c>
       <c r="E98">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1149.952348250544</v>
       </c>
     </row>
-    <row r="99" spans="3:5">
+    <row r="99" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C99" s="1">
         <v>0.20434723806894195</v>
       </c>
       <c r="D99">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.7431090045161537</v>
       </c>
       <c r="E99">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1152.6954572550601</v>
       </c>
     </row>
-    <row r="100" spans="3:5">
+    <row r="100" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C100" s="1">
         <v>0.12653066421940684</v>
       </c>
       <c r="D100">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6233870603168454</v>
       </c>
       <c r="E100">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1154.318844315377</v>
       </c>
     </row>
-    <row r="101" spans="3:5">
+    <row r="101" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C101" s="1">
         <v>0.4055260687667217</v>
       </c>
       <c r="D101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.2409409645764784</v>
       </c>
       <c r="E101">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1160.5597852799535</v>
       </c>
     </row>
-    <row r="102" spans="3:5">
+    <row r="102" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C102" s="1">
         <v>0.3477813378412129</v>
       </c>
       <c r="D102">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.128504822448666</v>
       </c>
       <c r="E102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1165.6882901024021</v>
       </c>
     </row>
-    <row r="103" spans="3:5">
+    <row r="103" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C103" s="1">
         <v>0.36358394997344012</v>
       </c>
       <c r="D103">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.4228331536883321</v>
       </c>
       <c r="E103">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1171.1111232560904</v>
       </c>
     </row>
-    <row r="104" spans="3:5">
+    <row r="104" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C104" s="1">
         <v>0.22118525141641721</v>
       </c>
       <c r="D104">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.9997848170582104</v>
       </c>
       <c r="E104">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1174.1109080731487</v>
       </c>
     </row>
-    <row r="105" spans="3:5">
+    <row r="105" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C105" s="1">
         <v>0.4513676075322981</v>
       </c>
       <c r="D105">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.203919878333731</v>
       </c>
       <c r="E105">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1181.3148279514824</v>
       </c>
     </row>
-    <row r="106" spans="3:5">
+    <row r="106" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C106" s="1">
         <v>0.71772828014354051</v>
       </c>
       <c r="D106">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>15.178621516389809</v>
       </c>
       <c r="E106">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1196.4934494678721</v>
       </c>
     </row>
-    <row r="107" spans="3:5">
+    <row r="107" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C107" s="1">
         <v>0.13186316214276617</v>
       </c>
       <c r="D107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6968711533502741</v>
       </c>
       <c r="E107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1198.1903206212223</v>
       </c>
     </row>
-    <row r="108" spans="3:5">
+    <row r="108" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C108" s="1">
         <v>0.75240251656148494</v>
       </c>
       <c r="D108">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16.751410824503356</v>
       </c>
       <c r="E108">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1214.9417314457257</v>
       </c>
     </row>
-    <row r="109" spans="3:5">
+    <row r="109" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C109" s="1">
         <v>5.2303200570330111E-2</v>
       </c>
       <c r="D109">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.64464791651357123</v>
       </c>
       <c r="E109">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1215.5863793622393</v>
       </c>
     </row>
-    <row r="110" spans="3:5">
+    <row r="110" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C110" s="1">
         <v>0.201626168370588</v>
       </c>
       <c r="D110">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.7021399664475245</v>
       </c>
       <c r="E110">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1218.2885193286868</v>
       </c>
     </row>
-    <row r="111" spans="3:5">
+    <row r="111" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C111" s="1">
         <v>0.96689065893020043</v>
       </c>
       <c r="D111">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>40.895277946384375</v>
       </c>
       <c r="E111">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1259.1837972750711</v>
       </c>
     </row>
-    <row r="112" spans="3:5">
+    <row r="112" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C112" s="1">
         <v>0.48407922076095389</v>
       </c>
       <c r="D112">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.9416246467255638</v>
       </c>
       <c r="E112">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1267.1254219217967</v>
       </c>
     </row>
-    <row r="113" spans="3:5">
+    <row r="113" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C113" s="1">
         <v>1.380996965474246E-2</v>
       </c>
       <c r="D113">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.16687457285250945</v>
       </c>
       <c r="E113">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1267.2922964946492</v>
       </c>
     </row>
-    <row r="114" spans="3:5">
+    <row r="114" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C114" s="1">
         <v>0.16993570445994699</v>
       </c>
       <c r="D114">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.2350254002275047</v>
       </c>
       <c r="E114">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1269.5273218948766</v>
       </c>
     </row>
-    <row r="115" spans="3:5">
+    <row r="115" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C115" s="1">
         <v>2.8350187309235331E-2</v>
       </c>
       <c r="D115">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.34511777334998955</v>
       </c>
       <c r="E115">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1269.8724396682267</v>
       </c>
     </row>
-    <row r="116" spans="3:5">
+    <row r="116" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C116" s="1">
         <v>5.0784510269774152E-2</v>
       </c>
       <c r="D116">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.62543322998893514</v>
       </c>
       <c r="E116">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1270.4978728982155</v>
       </c>
     </row>
-    <row r="117" spans="3:5">
+    <row r="117" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C117" s="1">
         <v>0.78976079445416136</v>
       </c>
       <c r="D117">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>18.714111869873527</v>
       </c>
       <c r="E117">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1289.211984768089</v>
       </c>
     </row>
-    <row r="118" spans="3:5">
+    <row r="118" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C118" s="1">
         <v>0.26574081431649876</v>
       </c>
       <c r="D118">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.7067183842497755</v>
       </c>
       <c r="E118">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1292.9187031523388</v>
       </c>
     </row>
-    <row r="119" spans="3:5">
+    <row r="119" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C119" s="1">
         <v>0.21603648744874526</v>
       </c>
       <c r="D119">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.9207135979353924</v>
       </c>
       <c r="E119">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1295.8394167502743</v>
       </c>
     </row>
-    <row r="120" spans="3:5">
+    <row r="120" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C120" s="1">
         <v>0.4436047667881855</v>
       </c>
       <c r="D120">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.0353166339937161</v>
       </c>
       <c r="E120">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1302.874733384268</v>
       </c>
     </row>
-    <row r="121" spans="3:5">
+    <row r="121" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C121" s="1">
         <v>0.25303521234761939</v>
       </c>
       <c r="D121">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.5008467997271211</v>
       </c>
       <c r="E121">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1306.375580183995</v>
       </c>
     </row>
-    <row r="122" spans="3:5">
+    <row r="122" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C122" s="1">
         <v>0.59945528392043101</v>
       </c>
       <c r="D122">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10.979158416846762</v>
       </c>
       <c r="E122">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1317.3547386008418</v>
       </c>
     </row>
-    <row r="123" spans="3:5">
+    <row r="123" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C123" s="1">
         <v>0.44195721404311428</v>
       </c>
       <c r="D123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.99983570637953</v>
       </c>
       <c r="E123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1324.3545743072214</v>
       </c>
     </row>
-    <row r="124" spans="3:5">
+    <row r="124" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C124" s="1">
         <v>0.1189570832555491</v>
       </c>
       <c r="D124">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.5197872867330739</v>
       </c>
       <c r="E124">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1325.8743615939545</v>
       </c>
     </row>
-    <row r="125" spans="3:5">
+    <row r="125" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C125" s="1">
         <v>0.47841837337149373</v>
       </c>
       <c r="D125">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.8106739281457402</v>
       </c>
       <c r="E125">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1333.6850355221002</v>
       </c>
     </row>
-    <row r="126" spans="3:5">
+    <row r="126" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C126" s="1">
         <v>0.66484083109463588</v>
       </c>
       <c r="D126">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13.117796747223647</v>
       </c>
       <c r="E126">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1346.8028322693237</v>
       </c>
     </row>
-    <row r="127" spans="3:5">
+    <row r="127" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C127" s="1">
         <v>0.73984162612473181</v>
       </c>
       <c r="D127">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16.157576437460019</v>
       </c>
       <c r="E127">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1362.9604087067837</v>
       </c>
     </row>
-    <row r="128" spans="3:5">
+    <row r="128" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C128" s="1">
         <v>0.79596820461425111</v>
       </c>
       <c r="D128">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>19.073753250584687</v>
       </c>
       <c r="E128">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1382.0341619573685</v>
       </c>
     </row>
-    <row r="129" spans="3:5">
+    <row r="129" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C129" s="1">
         <v>0.70569321036603383</v>
       </c>
       <c r="D129">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14.677590642684287</v>
       </c>
       <c r="E129">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1396.7117526000527</v>
       </c>
     </row>
-    <row r="130" spans="3:5">
+    <row r="130" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C130" s="1">
         <v>0.39917803977676858</v>
       </c>
       <c r="D130">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.1134795307640379</v>
       </c>
       <c r="E130">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1402.8252321308166</v>
       </c>
     </row>
-    <row r="131" spans="3:5">
+    <row r="131" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C131" s="1">
         <v>0.6892227375594846</v>
       </c>
       <c r="D131">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14.024145856027609</v>
       </c>
       <c r="E131">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1416.8493779868443</v>
       </c>
     </row>
-    <row r="132" spans="3:5">
+    <row r="132" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C132" s="1">
         <v>0.20288275469927375</v>
       </c>
       <c r="D132">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.721042032751829</v>
       </c>
       <c r="E132">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1419.5704200195962</v>
       </c>
     </row>
-    <row r="133" spans="3:5">
+    <row r="133" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C133" s="1">
         <v>0.75358468184308158</v>
       </c>
       <c r="D133">
-        <f t="shared" ref="D133:D196" si="8">-12*LN(1-C133)</f>
+        <f t="shared" ref="D133:D196" si="9">-12*LN(1-C133)</f>
         <v>16.808842576925716</v>
       </c>
       <c r="E133">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1436.379262596522</v>
       </c>
     </row>
-    <row r="134" spans="3:5">
+    <row r="134" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C134" s="1">
         <v>0.91340059598367063</v>
       </c>
       <c r="D134">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>29.357548145591494</v>
       </c>
       <c r="E134">
-        <f t="shared" ref="E134:E197" si="9">D134+E133</f>
+        <f t="shared" ref="E134:E197" si="10">D134+E133</f>
         <v>1465.7368107421134</v>
       </c>
     </row>
-    <row r="135" spans="3:5">
+    <row r="135" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C135" s="1">
         <v>0.75046206779022828</v>
       </c>
       <c r="D135">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>16.657732109297974</v>
       </c>
       <c r="E135">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1482.3945428514114</v>
       </c>
     </row>
-    <row r="136" spans="3:5">
+    <row r="136" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C136" s="1">
         <v>0.77791355452253885</v>
       </c>
       <c r="D136">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>18.0562629463371</v>
       </c>
       <c r="E136">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1500.4508057977484</v>
       </c>
     </row>
-    <row r="137" spans="3:5">
+    <row r="137" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C137" s="1">
         <v>0.76940749589827573</v>
       </c>
       <c r="D137">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>17.605238132869843</v>
       </c>
       <c r="E137">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1518.0560439306182</v>
       </c>
     </row>
-    <row r="138" spans="3:5">
+    <row r="138" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C138" s="1">
         <v>6.9870947856016663E-2</v>
       </c>
       <c r="D138">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.8691832405883082</v>
       </c>
       <c r="E138">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1518.9252271712064</v>
       </c>
     </row>
-    <row r="139" spans="3:5">
+    <row r="139" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C139" s="1">
         <v>0.71960070866676418</v>
       </c>
       <c r="D139">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>15.258487814005633</v>
       </c>
       <c r="E139">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1534.183714985212</v>
       </c>
     </row>
-    <row r="140" spans="3:5">
+    <row r="140" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C140" s="1">
         <v>0.75868312679900995</v>
       </c>
       <c r="D140">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>17.059732590706417</v>
       </c>
       <c r="E140">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1551.2434475759185</v>
       </c>
     </row>
-    <row r="141" spans="3:5">
+    <row r="141" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C141" s="1">
         <v>0.8678498503201153</v>
       </c>
       <c r="D141">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>24.285798063372766</v>
       </c>
       <c r="E141">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1575.5292456392913</v>
       </c>
     </row>
-    <row r="142" spans="3:5">
+    <row r="142" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C142" s="1">
         <v>0.2859962634026143</v>
       </c>
       <c r="D142">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.0424049999188956</v>
       </c>
       <c r="E142">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1579.5716506392102</v>
       </c>
     </row>
-    <row r="143" spans="3:5">
+    <row r="143" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C143" s="1">
         <v>0.58978429041601199</v>
       </c>
       <c r="D143">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10.692865640403872</v>
       </c>
       <c r="E143">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1590.2645162796141</v>
       </c>
     </row>
-    <row r="144" spans="3:5">
+    <row r="144" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C144" s="1">
         <v>0.81904693830324438</v>
       </c>
       <c r="D144">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>20.514211307877275</v>
       </c>
       <c r="E144">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1610.7787275874914</v>
       </c>
     </row>
-    <row r="145" spans="3:5">
+    <row r="145" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C145" s="1">
         <v>0.71704983786177401</v>
       </c>
       <c r="D145">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>15.149814028391196</v>
       </c>
       <c r="E145">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1625.9285416158825</v>
       </c>
     </row>
-    <row r="146" spans="3:5">
+    <row r="146" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C146" s="1">
         <v>0.5243630268419972</v>
       </c>
       <c r="D146">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8.917204525892009</v>
       </c>
       <c r="E146">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1634.8457461417745</v>
       </c>
     </row>
-    <row r="147" spans="3:5">
+    <row r="147" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C147" s="1">
         <v>0.46969763946945697</v>
       </c>
       <c r="D147">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7.6116953224482824</v>
       </c>
       <c r="E147">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1642.4574414642227</v>
       </c>
     </row>
-    <row r="148" spans="3:5">
+    <row r="148" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C148" s="1">
         <v>0.88219991304465584</v>
       </c>
       <c r="D148">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>25.665195235249286</v>
       </c>
       <c r="E148">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1668.122636699472</v>
       </c>
     </row>
-    <row r="149" spans="3:5">
+    <row r="149" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C149" s="1">
         <v>0.43499536483632983</v>
       </c>
       <c r="D149">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.8510561284781115</v>
       </c>
       <c r="E149">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1674.9736928279501</v>
       </c>
     </row>
-    <row r="150" spans="3:5">
+    <row r="150" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C150" s="1">
         <v>0.54500126455225506</v>
       </c>
       <c r="D150">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9.4495276712492888</v>
       </c>
       <c r="E150">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1684.4232204991995</v>
       </c>
     </row>
-    <row r="151" spans="3:5">
+    <row r="151" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C151" s="1">
         <v>0.50687624796219666</v>
       </c>
       <c r="D151">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8.4839414172842282</v>
       </c>
       <c r="E151">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1692.9071619164838</v>
       </c>
     </row>
-    <row r="152" spans="3:5">
+    <row r="152" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C152" s="1">
         <v>0.464477938198808</v>
       </c>
       <c r="D152">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7.4941582972160852</v>
       </c>
       <c r="E152">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1700.4013202136998</v>
       </c>
     </row>
-    <row r="153" spans="3:5">
+    <row r="153" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C153" s="1">
         <v>0.24233975560479237</v>
       </c>
       <c r="D153">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.3302426425774616</v>
       </c>
       <c r="E153">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1703.7315628562774</v>
       </c>
     </row>
-    <row r="154" spans="3:5">
+    <row r="154" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C154" s="1">
         <v>0.39925084439658498</v>
       </c>
       <c r="D154">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.1149337192466984</v>
       </c>
       <c r="E154">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1709.846496575524</v>
       </c>
     </row>
-    <row r="155" spans="3:5">
+    <row r="155" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C155" s="1">
         <v>5.0429601469931917E-2</v>
       </c>
       <c r="D155">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.62094730487854144</v>
       </c>
       <c r="E155">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1710.4674438804027</v>
       </c>
     </row>
-    <row r="156" spans="3:5">
+    <row r="156" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C156" s="1">
         <v>0.55397299118440846</v>
       </c>
       <c r="D156">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9.6885092509576225</v>
       </c>
       <c r="E156">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1720.1559531313603</v>
       </c>
     </row>
-    <row r="157" spans="3:5">
+    <row r="157" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C157" s="1">
         <v>4.7494370254120399E-2</v>
       </c>
       <c r="D157">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.58391113805263362</v>
       </c>
       <c r="E157">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1720.7398642694129</v>
       </c>
     </row>
-    <row r="158" spans="3:5">
+    <row r="158" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C158" s="1">
         <v>0.8943964264937323</v>
       </c>
       <c r="D158">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>26.976756819132746</v>
       </c>
       <c r="E158">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1747.7166210885457</v>
       </c>
     </row>
-    <row r="159" spans="3:5">
+    <row r="159" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C159" s="1">
         <v>0.759271150705354</v>
       </c>
       <c r="D159">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>17.089009026724163</v>
       </c>
       <c r="E159">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1764.8056301152699</v>
       </c>
     </row>
-    <row r="160" spans="3:5">
+    <row r="160" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C160" s="1">
         <v>4.7632933805275002E-3</v>
       </c>
       <c r="D160">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.729608819634445E-2</v>
       </c>
       <c r="E160">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1764.8629262034663</v>
       </c>
     </row>
-    <row r="161" spans="3:5">
+    <row r="161" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C161" s="1">
         <v>1.3175599269890093E-2</v>
       </c>
       <c r="D161">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.15915801005332364</v>
       </c>
       <c r="E161">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1765.0220842135195</v>
       </c>
     </row>
-    <row r="162" spans="3:5">
+    <row r="162" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C162" s="1">
         <v>0.31940083222480453</v>
       </c>
       <c r="D162">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.617380876365937</v>
       </c>
       <c r="E162">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1769.6394650898856</v>
       </c>
     </row>
-    <row r="163" spans="3:5">
+    <row r="163" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C163" s="1">
         <v>0.22262937250184689</v>
       </c>
       <c r="D163">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.0220565312973937</v>
       </c>
       <c r="E163">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1772.6615216211831</v>
       </c>
     </row>
-    <row r="164" spans="3:5">
+    <row r="164" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C164" s="1">
         <v>0.75973854491501314</v>
       </c>
       <c r="D164">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>17.112330628969435</v>
       </c>
       <c r="E164">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1789.7738522501525</v>
       </c>
     </row>
-    <row r="165" spans="3:5">
+    <row r="165" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C165" s="1">
         <v>0.84427331575125564</v>
       </c>
       <c r="D165">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>22.315833988419158</v>
       </c>
       <c r="E165">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1812.0896862385716</v>
       </c>
     </row>
-    <row r="166" spans="3:5">
+    <row r="166" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C166" s="1">
         <v>0.68912527732016482</v>
       </c>
       <c r="D166">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>14.02038322706667</v>
       </c>
       <c r="E166">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1826.1100694656384</v>
       </c>
     </row>
-    <row r="167" spans="3:5">
+    <row r="167" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C167" s="1">
         <v>5.7893094543596924E-2</v>
       </c>
       <c r="D167">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.71563827719244233</v>
       </c>
       <c r="E167">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1826.8257077428309</v>
       </c>
     </row>
-    <row r="168" spans="3:5">
+    <row r="168" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C168" s="1">
         <v>0.99775231863792802</v>
       </c>
       <c r="D168">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>73.174273198172401</v>
       </c>
       <c r="E168">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1899.9999809410033</v>
       </c>
     </row>
-    <row r="169" spans="3:5">
+    <row r="169" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C169" s="1">
         <v>0.32864189482359696</v>
       </c>
       <c r="D169">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.7814311470101778</v>
       </c>
       <c r="E169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1904.7814120880134</v>
       </c>
     </row>
-    <row r="170" spans="3:5">
+    <row r="170" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C170" s="1">
         <v>0.85281212055499922</v>
       </c>
       <c r="D170">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>22.992545001653301</v>
       </c>
       <c r="E170">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1927.7739570896667</v>
       </c>
     </row>
-    <row r="171" spans="3:5">
+    <row r="171" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C171" s="1">
         <v>0.3220602106586643</v>
       </c>
       <c r="D171">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.6643616151976222</v>
       </c>
       <c r="E171">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1932.4383187048643</v>
       </c>
     </row>
-    <row r="172" spans="3:5">
+    <row r="172" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C172" s="1">
         <v>0.99166829653265598</v>
       </c>
       <c r="D172">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>57.452248149957512</v>
       </c>
       <c r="E172">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1989.8905668548218</v>
       </c>
     </row>
-    <row r="173" spans="3:5">
+    <row r="173" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C173" s="1">
         <v>0.53957050922865779</v>
       </c>
       <c r="D173">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9.3071465941566576</v>
       </c>
       <c r="E173">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1999.1977134489784</v>
       </c>
     </row>
-    <row r="174" spans="3:5">
+    <row r="174" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C174" s="1">
         <v>0.84048501299334077</v>
       </c>
       <c r="D174">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>22.027408784966809</v>
       </c>
       <c r="E174">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2021.2251222339453</v>
       </c>
     </row>
-    <row r="175" spans="3:5">
+    <row r="175" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C175" s="1">
         <v>0.72849363235312481</v>
       </c>
       <c r="D175">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>15.645236235642326</v>
       </c>
       <c r="E175">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2036.8703584695877</v>
       </c>
     </row>
-    <row r="176" spans="3:5">
+    <row r="176" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C176" s="1">
         <v>0.90703539315706294</v>
       </c>
       <c r="D176">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>28.50643715815135</v>
       </c>
       <c r="E176">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2065.3767956277388</v>
       </c>
     </row>
-    <row r="177" spans="3:5">
+    <row r="177" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C177" s="1">
         <v>0.80780440851386381</v>
       </c>
       <c r="D177">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>19.790900637910582</v>
       </c>
       <c r="E177">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2085.1676962656493</v>
       </c>
     </row>
-    <row r="178" spans="3:5">
+    <row r="178" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C178" s="1">
         <v>0.42066748381293717</v>
       </c>
       <c r="D178">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.5505440678405034</v>
       </c>
       <c r="E178">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2091.7182403334896</v>
       </c>
     </row>
-    <row r="179" spans="3:5">
+    <row r="179" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C179" s="1">
         <v>0.1872961491074312</v>
       </c>
       <c r="D179">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.4886620340859187</v>
       </c>
       <c r="E179">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2094.2069023675754</v>
       </c>
     </row>
-    <row r="180" spans="3:5">
+    <row r="180" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C180" s="1">
         <v>0.31341147032225725</v>
       </c>
       <c r="D180">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.5122412488739938</v>
       </c>
       <c r="E180">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2098.7191436164494</v>
       </c>
     </row>
-    <row r="181" spans="3:5">
+    <row r="181" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C181" s="1">
         <v>0.70522870935580606</v>
       </c>
       <c r="D181">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>14.658666111405353</v>
       </c>
       <c r="E181">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2113.3778097278546</v>
       </c>
     </row>
-    <row r="182" spans="3:5">
+    <row r="182" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C182" s="1">
         <v>0.66575947750426145</v>
       </c>
       <c r="D182">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>13.150733015278647</v>
       </c>
       <c r="E182">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2126.5285427431331</v>
       </c>
     </row>
-    <row r="183" spans="3:5">
+    <row r="183" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C183" s="1">
         <v>0.29156396944136831</v>
       </c>
       <c r="D183">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.1363461497944609</v>
       </c>
       <c r="E183">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2130.6648888929276</v>
       </c>
     </row>
-    <row r="184" spans="3:5">
+    <row r="184" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C184" s="1">
         <v>0.64534253140799525</v>
       </c>
       <c r="D184">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>12.43923399007199</v>
       </c>
       <c r="E184">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2143.1041228829995</v>
       </c>
     </row>
-    <row r="185" spans="3:5">
+    <row r="185" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C185" s="1">
         <v>0.18074872912422624</v>
       </c>
       <c r="D185">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.3923732816448355</v>
       </c>
       <c r="E185">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2145.4964961646442</v>
       </c>
     </row>
-    <row r="186" spans="3:5">
+    <row r="186" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C186" s="1">
         <v>0.24979266110760978</v>
       </c>
       <c r="D186">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.4488679056124072</v>
       </c>
       <c r="E186">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2148.9453640702568</v>
       </c>
     </row>
-    <row r="187" spans="3:5">
+    <row r="187" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C187" s="1">
         <v>0.77261963527080013</v>
       </c>
       <c r="D187">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>17.773572578773148</v>
       </c>
       <c r="E187">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2166.7189366490297</v>
       </c>
     </row>
-    <row r="188" spans="3:5">
+    <row r="188" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C188" s="1">
         <v>0.26736567683203227</v>
       </c>
       <c r="D188">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.7333029427653335</v>
       </c>
       <c r="E188">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2170.4522395917952</v>
       </c>
     </row>
-    <row r="189" spans="3:5">
+    <row r="189" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C189" s="1">
         <v>0.63231135776904779</v>
       </c>
       <c r="D189">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>12.006225358029786</v>
       </c>
       <c r="E189">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2182.4584649498252</v>
       </c>
     </row>
-    <row r="190" spans="3:5">
+    <row r="190" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C190" s="1">
         <v>0.22696520786549357</v>
       </c>
       <c r="D190">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.0891746661356034</v>
       </c>
       <c r="E190">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2185.5476396159606</v>
       </c>
     </row>
-    <row r="191" spans="3:5">
+    <row r="191" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C191" s="1">
         <v>0.47591813245037717</v>
       </c>
       <c r="D191">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7.7532884529949273</v>
       </c>
       <c r="E191">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2193.3009280689557</v>
       </c>
     </row>
-    <row r="192" spans="3:5">
+    <row r="192" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C192" s="1">
         <v>0.96074927707580393</v>
       </c>
       <c r="D192">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>38.853424997669784</v>
       </c>
       <c r="E192">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2232.1543530666254</v>
       </c>
     </row>
-    <row r="193" spans="3:5">
+    <row r="193" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C193" s="1">
         <v>0.53008839746287162</v>
       </c>
       <c r="D193">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9.0625281801057191</v>
       </c>
       <c r="E193">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2241.2168812467312</v>
       </c>
     </row>
-    <row r="194" spans="3:5">
+    <row r="194" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C194" s="1">
         <v>0.53985190113487325</v>
       </c>
       <c r="D194">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9.3144826471255016</v>
       </c>
       <c r="E194">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2250.5313638938569</v>
       </c>
     </row>
-    <row r="195" spans="3:5">
+    <row r="195" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C195" s="1">
         <v>0.8128834262795408</v>
       </c>
       <c r="D195">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>20.112281609690669</v>
       </c>
       <c r="E195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2270.6436455035478</v>
       </c>
     </row>
-    <row r="196" spans="3:5">
+    <row r="196" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C196" s="1">
         <v>0.76878361481761548</v>
       </c>
       <c r="D196">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>17.572815294348757</v>
       </c>
       <c r="E196">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2288.2164607978966</v>
       </c>
     </row>
-    <row r="197" spans="3:5">
+    <row r="197" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C197" s="1">
         <v>0.96449957813804787</v>
       </c>
       <c r="D197">
-        <f t="shared" ref="D197:D253" si="10">-12*LN(1-C197)</f>
+        <f t="shared" ref="D197:D253" si="11">-12*LN(1-C197)</f>
         <v>40.058528389633238</v>
       </c>
       <c r="E197">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2328.2749891875301</v>
       </c>
     </row>
-    <row r="198" spans="3:5">
+    <row r="198" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C198" s="1">
         <v>0.72982025623583002</v>
       </c>
       <c r="D198">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15.704013885964615</v>
       </c>
       <c r="E198">
-        <f t="shared" ref="E198:E253" si="11">D198+E197</f>
+        <f t="shared" ref="E198:E253" si="12">D198+E197</f>
         <v>2343.9790030734948</v>
       </c>
     </row>
-    <row r="199" spans="3:5">
+    <row r="199" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C199" s="1">
         <v>0.49507778819526127</v>
       </c>
       <c r="D199">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8.2002107712211831</v>
       </c>
       <c r="E199">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2352.1792138447158</v>
       </c>
     </row>
-    <row r="200" spans="3:5">
+    <row r="200" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C200" s="1">
         <v>0.57598180758801498</v>
       </c>
       <c r="D200">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10.295747016463228</v>
       </c>
       <c r="E200">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2362.4749608611792</v>
       </c>
     </row>
-    <row r="201" spans="3:5">
+    <row r="201" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C201" s="1">
         <v>0.96389174517809195</v>
       </c>
       <c r="D201">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>39.854805292277284</v>
       </c>
       <c r="E201">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2402.3297661534566</v>
       </c>
     </row>
-    <row r="202" spans="3:5">
+    <row r="202" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C202" s="1">
         <v>0.71456768133950654</v>
       </c>
       <c r="D202">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15.045004085699539</v>
       </c>
       <c r="E202">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2417.3747702391561</v>
       </c>
     </row>
-    <row r="203" spans="3:5">
+    <row r="203" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C203" s="1">
         <v>0.55715825693157228</v>
       </c>
       <c r="D203">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.7745137426234319</v>
       </c>
       <c r="E203">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2427.1492839817797</v>
       </c>
     </row>
-    <row r="204" spans="3:5">
+    <row r="204" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C204" s="1">
         <v>0.96035960518409746</v>
       </c>
       <c r="D204">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>38.734879314384557</v>
       </c>
       <c r="E204">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2465.8841632961644</v>
       </c>
     </row>
-    <row r="205" spans="3:5">
+    <row r="205" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C205" s="1">
         <v>0.38890538982200606</v>
       </c>
       <c r="D205">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5.9100418438711309</v>
       </c>
       <c r="E205">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2471.7942051400355</v>
       </c>
     </row>
-    <row r="206" spans="3:5">
+    <row r="206" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C206" s="1">
         <v>0.63909076281890842</v>
       </c>
       <c r="D206">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>12.229545273740332</v>
       </c>
       <c r="E206">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2484.0237504137758</v>
       </c>
     </row>
-    <row r="207" spans="3:5">
+    <row r="207" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C207" s="1">
         <v>8.0911641020764868E-2</v>
       </c>
       <c r="D207">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0124761724646802</v>
       </c>
       <c r="E207">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2485.0362265862404</v>
       </c>
     </row>
-    <row r="208" spans="3:5">
+    <row r="208" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C208" s="1">
         <v>0.52992905080386854</v>
       </c>
       <c r="D208">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.0584596792110421</v>
       </c>
       <c r="E208">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2494.0946862654514</v>
       </c>
     </row>
-    <row r="209" spans="3:5">
+    <row r="209" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C209" s="1">
         <v>0.58140333800157706</v>
       </c>
       <c r="D209">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10.450169318466152</v>
       </c>
       <c r="E209">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2504.5448555839175</v>
       </c>
     </row>
-    <row r="210" spans="3:5">
+    <row r="210" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C210" s="1">
         <v>0.45780539916973506</v>
       </c>
       <c r="D210">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7.345563598325155</v>
       </c>
       <c r="E210">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2511.8904191822426</v>
       </c>
     </row>
-    <row r="211" spans="3:5">
+    <row r="211" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C211" s="1">
         <v>0.52872419672030713</v>
       </c>
       <c r="D211">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.0277414409849364</v>
       </c>
       <c r="E211">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2520.9181606232273</v>
       </c>
     </row>
-    <row r="212" spans="3:5">
+    <row r="212" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C212" s="1">
         <v>0.51712575485343137</v>
       </c>
       <c r="D212">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8.7359882549402901</v>
       </c>
       <c r="E212">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2529.6541488781677</v>
       </c>
     </row>
-    <row r="213" spans="3:5">
+    <row r="213" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C213" s="1">
         <v>0.83228001510195826</v>
       </c>
       <c r="D213">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>21.425513360667111</v>
       </c>
       <c r="E213">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2551.0796622388348</v>
       </c>
     </row>
-    <row r="214" spans="3:5">
+    <row r="214" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C214" s="1">
         <v>0.62079223701303299</v>
       </c>
       <c r="D214">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>11.636052441585303</v>
       </c>
       <c r="E214">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2562.7157146804202</v>
       </c>
     </row>
-    <row r="215" spans="3:5">
+    <row r="215" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C215" s="1">
         <v>0.25154679445676642</v>
       </c>
       <c r="D215">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.4769591366528867</v>
       </c>
       <c r="E215">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2566.1926738170732</v>
       </c>
     </row>
-    <row r="216" spans="3:5">
+    <row r="216" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C216" s="1">
         <v>0.95361204168821279</v>
       </c>
       <c r="D216">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>36.848584470880375</v>
       </c>
       <c r="E216">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2603.0412582879535</v>
       </c>
     </row>
-    <row r="217" spans="3:5">
+    <row r="217" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C217" s="1">
         <v>0.64819530229874678</v>
       </c>
       <c r="D217">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>12.536149121262223</v>
       </c>
       <c r="E217">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2615.5774074092155</v>
       </c>
     </row>
-    <row r="218" spans="3:5">
+    <row r="218" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C218" s="1">
         <v>0.95633073552027636</v>
       </c>
       <c r="D218">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>37.573329051799206</v>
       </c>
       <c r="E218">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2653.1507364610147</v>
       </c>
     </row>
-    <row r="219" spans="3:5">
+    <row r="219" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C219" s="1">
         <v>0.48428252665534388</v>
       </c>
       <c r="D219">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7.9463543487468939</v>
       </c>
       <c r="E219">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2661.0970908097615</v>
       </c>
     </row>
-    <row r="220" spans="3:5">
+    <row r="220" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C220" s="1">
         <v>0.41512762462502284</v>
       </c>
       <c r="D220">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6.4363394076383171</v>
       </c>
       <c r="E220">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2667.5334302173997</v>
       </c>
     </row>
-    <row r="221" spans="3:5">
+    <row r="221" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C221" s="1">
         <v>0.83847720342569554</v>
       </c>
       <c r="D221">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>21.87730789226449</v>
       </c>
       <c r="E221">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2689.4107381096642</v>
       </c>
     </row>
-    <row r="222" spans="3:5">
+    <row r="222" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C222" s="1">
         <v>0.75754654771836227</v>
       </c>
       <c r="D222">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>17.003346436599664</v>
       </c>
       <c r="E222">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2706.4140845462639</v>
       </c>
     </row>
-    <row r="223" spans="3:5">
+    <row r="223" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C223" s="1">
         <v>0.71903520050588998</v>
       </c>
       <c r="D223">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15.234310634392866</v>
       </c>
       <c r="E223">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2721.6483951806567</v>
       </c>
     </row>
-    <row r="224" spans="3:5">
+    <row r="224" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C224" s="1">
         <v>0.52693141835073476</v>
       </c>
       <c r="D224">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8.9821788970160021</v>
       </c>
       <c r="E224">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2730.6305740776729</v>
       </c>
     </row>
-    <row r="225" spans="3:5">
+    <row r="225" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C225" s="1">
         <v>0.54057269311730471</v>
       </c>
       <c r="D225">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.3332946020919074</v>
       </c>
       <c r="E225">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2739.9638686797648</v>
       </c>
     </row>
-    <row r="226" spans="3:5">
+    <row r="226" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C226" s="1">
         <v>0.56852361779920502</v>
       </c>
       <c r="D226">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10.086510049654372</v>
       </c>
       <c r="E226">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2750.0503787294192</v>
       </c>
     </row>
-    <row r="227" spans="3:5">
+    <row r="227" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C227" s="1">
         <v>0.21833855860448281</v>
       </c>
       <c r="D227">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.956002858888775</v>
       </c>
       <c r="E227">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2753.0063815883082</v>
       </c>
     </row>
-    <row r="228" spans="3:5">
+    <row r="228" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C228" s="1">
         <v>0.20977720026382496</v>
       </c>
       <c r="D228">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.8252841796016748</v>
       </c>
       <c r="E228">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2755.8316657679097</v>
       </c>
     </row>
-    <row r="229" spans="3:5">
+    <row r="229" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C229" s="1">
         <v>0.96775933298920691</v>
       </c>
       <c r="D229">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>41.214320071648089</v>
       </c>
       <c r="E229">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2797.0459858395579</v>
       </c>
     </row>
-    <row r="230" spans="3:5">
+    <row r="230" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C230" s="1">
         <v>0.43992807294460157</v>
       </c>
       <c r="D230">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6.9562807479653852</v>
       </c>
       <c r="E230">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2804.0022665875235</v>
       </c>
     </row>
-    <row r="231" spans="3:5">
+    <row r="231" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C231" s="1">
         <v>0.27470605457216735</v>
       </c>
       <c r="D231">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.8541391719290883</v>
       </c>
       <c r="E231">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2807.8564057594526</v>
       </c>
     </row>
-    <row r="232" spans="3:5">
+    <row r="232" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C232" s="1">
         <v>0.37232732859587436</v>
       </c>
       <c r="D232">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5.5888376673252553</v>
       </c>
       <c r="E232">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2813.4452434267778</v>
       </c>
     </row>
-    <row r="233" spans="3:5">
+    <row r="233" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C233" s="1">
         <v>0.89551031864016917</v>
       </c>
       <c r="D233">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>27.104003465049658</v>
       </c>
       <c r="E233">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2840.5492468918274</v>
       </c>
     </row>
-    <row r="234" spans="3:5">
+    <row r="234" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C234" s="1">
         <v>0.17683698637815759</v>
       </c>
       <c r="D234">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.3352123056916119</v>
       </c>
       <c r="E234">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2842.8844591975189</v>
       </c>
     </row>
-    <row r="235" spans="3:5">
+    <row r="235" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C235" s="1">
         <v>0.51057422035110189</v>
       </c>
       <c r="D235">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8.5742694399752981</v>
       </c>
       <c r="E235">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2851.4587286374945</v>
       </c>
     </row>
-    <row r="236" spans="3:5">
+    <row r="236" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C236" s="1">
         <v>0.13362900493883689</v>
       </c>
       <c r="D236">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.7213047367237022</v>
       </c>
       <c r="E236">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2853.1800333742181</v>
       </c>
     </row>
-    <row r="237" spans="3:5">
+    <row r="237" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C237" s="1">
         <v>0.19784999079948129</v>
       </c>
       <c r="D237">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.6455157365827491</v>
       </c>
       <c r="E237">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2855.8255491108007</v>
       </c>
     </row>
-    <row r="238" spans="3:5">
+    <row r="238" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C238" s="1">
         <v>0.6135491835170841</v>
       </c>
       <c r="D238">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>11.409008071846284</v>
       </c>
       <c r="E238">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2867.2345571826468</v>
       </c>
     </row>
-    <row r="239" spans="3:5">
+    <row r="239" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C239" s="1">
         <v>0.13225142111886434</v>
       </c>
       <c r="D239">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.7022391433638377</v>
       </c>
       <c r="E239">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2868.9367963260106</v>
       </c>
     </row>
-    <row r="240" spans="3:5">
+    <row r="240" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C240" s="1">
         <v>0.33493991460688854</v>
       </c>
       <c r="D240">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.8945346612002449</v>
       </c>
       <c r="E240">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2873.831330987211</v>
       </c>
     </row>
-    <row r="241" spans="3:5">
+    <row r="241" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C241" s="1">
         <v>9.2008963894674167E-4</v>
       </c>
       <c r="D241">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.1046158174837216E-2</v>
       </c>
       <c r="E241">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2873.8423771453859</v>
       </c>
     </row>
-    <row r="242" spans="3:5">
+    <row r="242" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C242" s="1">
         <v>0.23221979952220217</v>
       </c>
       <c r="D242">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.1710214090951245</v>
       </c>
       <c r="E242">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2877.0133985544808</v>
       </c>
     </row>
-    <row r="243" spans="3:5">
+    <row r="243" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C243" s="1">
         <v>0.84529937086410301</v>
       </c>
       <c r="D243">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>22.395161455186379</v>
       </c>
       <c r="E243">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2899.4085600096673</v>
       </c>
     </row>
-    <row r="244" spans="3:5">
+    <row r="244" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C244" s="1">
         <v>0.81499307421547051</v>
       </c>
       <c r="D244">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>20.248344215176974</v>
       </c>
       <c r="E244">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2919.6569042248443</v>
       </c>
     </row>
-    <row r="245" spans="3:5">
+    <row r="245" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C245" s="1">
         <v>0.74321006046775917</v>
       </c>
       <c r="D245">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>16.313962610520747</v>
       </c>
       <c r="E245">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2935.9708668353651</v>
       </c>
     </row>
-    <row r="246" spans="3:5">
+    <row r="246" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C246" s="1">
         <v>7.2152201986112274E-2</v>
       </c>
       <c r="D246">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.89865084489682745</v>
       </c>
       <c r="E246">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2936.8695176802621</v>
       </c>
     </row>
-    <row r="247" spans="3:5">
+    <row r="247" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C247" s="1">
         <v>0.46161181057555556</v>
       </c>
       <c r="D247">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7.4301052479033443</v>
       </c>
       <c r="E247">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2944.2996229281653</v>
       </c>
     </row>
-    <row r="248" spans="3:5">
+    <row r="248" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C248" s="1">
         <v>3.1365973292964533E-2</v>
       </c>
       <c r="D248">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.38242103817417844</v>
       </c>
       <c r="E248">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2944.6820439663393</v>
       </c>
     </row>
-    <row r="249" spans="3:5">
+    <row r="249" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C249" s="1">
         <v>0.86272034875874759</v>
       </c>
       <c r="D249">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>23.828822204853054</v>
       </c>
       <c r="E249">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2968.5108661711924</v>
       </c>
     </row>
-    <row r="250" spans="3:5">
+    <row r="250" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C250" s="1">
         <v>0.67618026150349753</v>
       </c>
       <c r="D250">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>13.530819368184725</v>
       </c>
       <c r="E250">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2982.0416855393773</v>
       </c>
     </row>
-    <row r="251" spans="3:5">
+    <row r="251" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C251" s="1">
         <v>0.83219736991534177</v>
       </c>
       <c r="D251">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>21.419601733759301</v>
       </c>
       <c r="E251">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3003.4612872731368</v>
       </c>
     </row>
-    <row r="252" spans="3:5">
+    <row r="252" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C252" s="1">
         <v>3.4087460044460727E-2</v>
       </c>
       <c r="D252">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.41618384660118901</v>
       </c>
       <c r="E252">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3003.8774711197379</v>
       </c>
     </row>
-    <row r="253" spans="3:5">
+    <row r="253" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C253" s="1">
         <v>0.80053428429387541</v>
       </c>
       <c r="D253">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19.345354902209166</v>
       </c>
       <c r="E253">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3023.2228260219472</v>
       </c>
     </row>
@@ -4681,24 +4773,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>